<commit_message>
Use titration curves from Atle
</commit_message>
<xml_diff>
--- a/data/titration_curves_atle_hindar.xlsx
+++ b/data/titration_curves_atle_hindar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E63671E-F440-45E9-8D9F-6CB7CC50E4A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4F9E0D-B096-4107-A2A5-B570A8190A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6FC24E5B-EEFC-4169-9832-26FC1932CCD3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6FC24E5B-EEFC-4169-9832-26FC1932CCD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -101,12 +106,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,778 +429,777 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>4.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
         <v>0.1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <f t="shared" ref="C3:C22" si="0">C2+0.1</f>
         <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
         <v>0.2</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <f t="shared" si="0"/>
         <v>4.6999999999999993</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
         <v>0.3</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <f t="shared" si="0"/>
         <v>4.7999999999999989</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
         <v>0.4</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <f t="shared" si="0"/>
         <v>4.8999999999999986</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
         <v>0.5</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <f t="shared" si="0"/>
         <v>4.9999999999999982</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
         <v>0.6</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <f t="shared" si="0"/>
         <v>5.0999999999999979</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
         <v>0.72</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>5.1999999999999975</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
         <v>0.84</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>5.2999999999999972</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
         <v>0.96</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <f t="shared" si="0"/>
         <v>5.3999999999999968</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
         <v>1.08</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <f t="shared" si="0"/>
         <v>5.4999999999999964</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="2">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
         <v>1.2</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <f t="shared" si="0"/>
         <v>5.5999999999999961</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
         <v>1.33</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <f t="shared" si="0"/>
         <v>5.6999999999999957</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
         <v>1.46</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <f t="shared" si="0"/>
         <v>5.7999999999999954</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
         <v>1.58</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <f t="shared" si="0"/>
         <v>5.899999999999995</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
         <v>1.7</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <f t="shared" si="0"/>
         <v>5.9999999999999947</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1">
         <v>1.85</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <f t="shared" si="0"/>
         <v>6.0999999999999943</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="2">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
         <f t="shared" si="0"/>
         <v>6.199999999999994</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="2">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
         <v>2.15</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <f t="shared" si="0"/>
         <v>6.2999999999999936</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="2">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <f t="shared" si="0"/>
         <v>6.3999999999999932</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1">
         <v>2.5</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <f t="shared" si="0"/>
         <v>6.4999999999999929</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="2">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1">
         <v>0</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>4.5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="2">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1">
         <v>0.1</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <f t="shared" ref="C24:C43" si="1">C23+0.1</f>
         <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="2">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1">
         <v>0.2</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <f t="shared" si="1"/>
         <v>4.6999999999999993</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="2">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="1">
         <v>0.3</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <f t="shared" si="1"/>
         <v>4.7999999999999989</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="2">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1">
         <v>0.4</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <f t="shared" si="1"/>
         <v>4.8999999999999986</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="2">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <f t="shared" si="1"/>
         <v>4.9999999999999982</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" s="2">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1">
         <v>0.65</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <f t="shared" si="1"/>
         <v>5.0999999999999979</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" s="2">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1">
         <v>0.78</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <f t="shared" si="1"/>
         <v>5.1999999999999975</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="2">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1">
         <v>0.92</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <f t="shared" si="1"/>
         <v>5.2999999999999972</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="2">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1">
         <v>1.05</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <f t="shared" si="1"/>
         <v>5.3999999999999968</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="2">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="1">
         <v>1.2</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <f t="shared" si="1"/>
         <v>5.4999999999999964</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" s="2">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1">
         <v>1.36</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <f t="shared" si="1"/>
         <v>5.5999999999999961</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="2">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="1">
         <v>1.5</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <f t="shared" si="1"/>
         <v>5.6999999999999957</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="2">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="1">
         <v>1.64</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <f t="shared" si="1"/>
         <v>5.7999999999999954</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="2">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="1">
         <v>1.79</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="1">
         <f t="shared" si="1"/>
         <v>5.899999999999995</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="2">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="1">
         <v>1.94</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="1">
         <f t="shared" si="1"/>
         <v>5.9999999999999947</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="2">
+      <c r="A39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="1">
         <v>2.1</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="1">
         <f t="shared" si="1"/>
         <v>6.0999999999999943</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="2">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="1">
         <v>2.2799999999999998</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="1">
         <f t="shared" si="1"/>
         <v>6.199999999999994</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="2">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1">
         <v>2.4500000000000002</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="1">
         <f t="shared" si="1"/>
         <v>6.2999999999999936</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" s="2">
+      <c r="A42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="1">
         <v>2.62</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <f t="shared" si="1"/>
         <v>6.3999999999999932</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="2">
+      <c r="A43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="1">
         <v>2.8</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="1">
         <f t="shared" si="1"/>
         <v>6.4999999999999929</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="2">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="1">
         <v>0</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="1">
         <v>4.5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B45" s="2">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="1">
         <v>0.1</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="1">
         <f t="shared" ref="C45:C64" si="2">C44+0.1</f>
         <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" s="2">
+      <c r="A46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="1">
         <v>0.2</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="1">
         <f t="shared" si="2"/>
         <v>4.6999999999999993</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B47" s="2">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="1">
         <v>0.3</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1">
         <f t="shared" si="2"/>
         <v>4.7999999999999989</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B48" s="2">
+      <c r="A48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="1">
         <v>0.4</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="1">
         <f t="shared" si="2"/>
         <v>4.8999999999999986</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B49" s="2">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="1">
         <f t="shared" si="2"/>
         <v>4.9999999999999982</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" s="2">
+      <c r="A50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="1">
         <v>0.7</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="1">
         <f t="shared" si="2"/>
         <v>5.0999999999999979</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B51" s="2">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1">
         <v>0.85</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="1">
         <f t="shared" si="2"/>
         <v>5.1999999999999975</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B52" s="2">
-        <v>1</v>
-      </c>
-      <c r="C52" s="2">
+      <c r="A52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1">
         <f t="shared" si="2"/>
         <v>5.2999999999999972</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B53" s="2">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="1">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="1">
         <f t="shared" si="2"/>
         <v>5.3999999999999968</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B54" s="2">
+      <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="1">
         <v>1.3</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="1">
         <f t="shared" si="2"/>
         <v>5.4999999999999964</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B55" s="2">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="1">
         <v>1.48</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="1">
         <f t="shared" si="2"/>
         <v>5.5999999999999961</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B56" s="2">
+      <c r="A56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="1">
         <v>1.64</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="1">
         <f t="shared" si="2"/>
         <v>5.6999999999999957</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B57" s="2">
+      <c r="A57" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="1">
         <v>1.8</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="1">
         <f t="shared" si="2"/>
         <v>5.7999999999999954</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B58" s="2">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="1">
         <v>1.96</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="1">
         <f t="shared" si="2"/>
         <v>5.899999999999995</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B59" s="2">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="1">
         <v>2.17</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="1">
         <f t="shared" si="2"/>
         <v>5.9999999999999947</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B60" s="2">
+      <c r="A60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="1">
         <v>2.35</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="1">
         <f t="shared" si="2"/>
         <v>6.0999999999999943</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B61" s="2">
+      <c r="A61" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="1">
         <v>2.58</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="1">
         <f t="shared" si="2"/>
         <v>6.199999999999994</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B62" s="2">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" s="1">
         <v>2.8</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="1">
         <f t="shared" si="2"/>
         <v>6.2999999999999936</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B63" s="2">
+      <c r="A63" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" s="1">
         <v>3.02</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="1">
         <f t="shared" si="2"/>
         <v>6.3999999999999932</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B64" s="2">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="1">
         <v>3.3</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="1">
         <f t="shared" si="2"/>
         <v>6.4999999999999929</v>
       </c>

</xml_diff>

<commit_message>
Add artificial endpoint to titration curves
For modelled CaCO3 concentrations outside the range of Atle's data, the model extrapolates, which can give unrealistic values for modelled pH. Instead, add an extreme artificial endpoint to the titration data based on a saturated solution of CaCO3 at room temperature and pressure (13 mg/l CaCO3 and pH 8.4). This is still not realistic, but at least constrains the model to physically plausible ranges of pH.
</commit_message>
<xml_diff>
--- a/data/titration_curves_atle_hindar.xlsx
+++ b/data/titration_curves_atle_hindar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4F9E0D-B096-4107-A2A5-B570A8190A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1650E2EC-2650-4300-A231-BF7560A8A991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6FC24E5B-EEFC-4169-9832-26FC1932CCD3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6FC24E5B-EEFC-4169-9832-26FC1932CCD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="6">
   <si>
     <t>pH</t>
   </si>
@@ -425,11 +425,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{087283B7-E47B-4E58-8DEA-50F4B5D6456F}">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,13 +704,13 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C23" s="1">
-        <v>4.5</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -718,11 +718,10 @@
         <v>2</v>
       </c>
       <c r="B24" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" ref="C24:C43" si="1">C23+0.1</f>
-        <v>4.5999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -730,11 +729,11 @@
         <v>2</v>
       </c>
       <c r="B25" s="1">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" si="1"/>
-        <v>4.6999999999999993</v>
+        <f t="shared" ref="C25:C44" si="1">C24+0.1</f>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -742,11 +741,11 @@
         <v>2</v>
       </c>
       <c r="B26" s="1">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" si="1"/>
-        <v>4.7999999999999989</v>
+        <v>4.6999999999999993</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -754,11 +753,11 @@
         <v>2</v>
       </c>
       <c r="B27" s="1">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" si="1"/>
-        <v>4.8999999999999986</v>
+        <v>4.7999999999999989</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -766,11 +765,11 @@
         <v>2</v>
       </c>
       <c r="B28" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.4</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" si="1"/>
-        <v>4.9999999999999982</v>
+        <v>4.8999999999999986</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -778,11 +777,11 @@
         <v>2</v>
       </c>
       <c r="B29" s="1">
-        <v>0.65</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" si="1"/>
-        <v>5.0999999999999979</v>
+        <v>4.9999999999999982</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -790,11 +789,11 @@
         <v>2</v>
       </c>
       <c r="B30" s="1">
-        <v>0.78</v>
+        <v>0.65</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" si="1"/>
-        <v>5.1999999999999975</v>
+        <v>5.0999999999999979</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -802,11 +801,11 @@
         <v>2</v>
       </c>
       <c r="B31" s="1">
-        <v>0.92</v>
+        <v>0.78</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" si="1"/>
-        <v>5.2999999999999972</v>
+        <v>5.1999999999999975</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -814,11 +813,11 @@
         <v>2</v>
       </c>
       <c r="B32" s="1">
-        <v>1.05</v>
+        <v>0.92</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" si="1"/>
-        <v>5.3999999999999968</v>
+        <v>5.2999999999999972</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -826,11 +825,11 @@
         <v>2</v>
       </c>
       <c r="B33" s="1">
-        <v>1.2</v>
+        <v>1.05</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" si="1"/>
-        <v>5.4999999999999964</v>
+        <v>5.3999999999999968</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -838,11 +837,11 @@
         <v>2</v>
       </c>
       <c r="B34" s="1">
-        <v>1.36</v>
+        <v>1.2</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" si="1"/>
-        <v>5.5999999999999961</v>
+        <v>5.4999999999999964</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -850,11 +849,11 @@
         <v>2</v>
       </c>
       <c r="B35" s="1">
-        <v>1.5</v>
+        <v>1.36</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" si="1"/>
-        <v>5.6999999999999957</v>
+        <v>5.5999999999999961</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -862,11 +861,11 @@
         <v>2</v>
       </c>
       <c r="B36" s="1">
-        <v>1.64</v>
+        <v>1.5</v>
       </c>
       <c r="C36" s="1">
         <f t="shared" si="1"/>
-        <v>5.7999999999999954</v>
+        <v>5.6999999999999957</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -874,11 +873,11 @@
         <v>2</v>
       </c>
       <c r="B37" s="1">
-        <v>1.79</v>
+        <v>1.64</v>
       </c>
       <c r="C37" s="1">
         <f t="shared" si="1"/>
-        <v>5.899999999999995</v>
+        <v>5.7999999999999954</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -886,11 +885,11 @@
         <v>2</v>
       </c>
       <c r="B38" s="1">
-        <v>1.94</v>
+        <v>1.79</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" si="1"/>
-        <v>5.9999999999999947</v>
+        <v>5.899999999999995</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -898,11 +897,11 @@
         <v>2</v>
       </c>
       <c r="B39" s="1">
-        <v>2.1</v>
+        <v>1.94</v>
       </c>
       <c r="C39" s="1">
         <f t="shared" si="1"/>
-        <v>6.0999999999999943</v>
+        <v>5.9999999999999947</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -910,11 +909,11 @@
         <v>2</v>
       </c>
       <c r="B40" s="1">
-        <v>2.2799999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="C40" s="1">
         <f t="shared" si="1"/>
-        <v>6.199999999999994</v>
+        <v>6.0999999999999943</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -922,11 +921,11 @@
         <v>2</v>
       </c>
       <c r="B41" s="1">
-        <v>2.4500000000000002</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="C41" s="1">
         <f t="shared" si="1"/>
-        <v>6.2999999999999936</v>
+        <v>6.199999999999994</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -934,11 +933,11 @@
         <v>2</v>
       </c>
       <c r="B42" s="1">
-        <v>2.62</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="C42" s="1">
         <f t="shared" si="1"/>
-        <v>6.3999999999999932</v>
+        <v>6.2999999999999936</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -946,34 +945,34 @@
         <v>2</v>
       </c>
       <c r="B43" s="1">
-        <v>2.8</v>
+        <v>2.62</v>
       </c>
       <c r="C43" s="1">
         <f t="shared" si="1"/>
-        <v>6.4999999999999929</v>
+        <v>6.3999999999999932</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B44" s="1">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="C44" s="1">
-        <v>4.5</v>
+        <f t="shared" si="1"/>
+        <v>6.4999999999999929</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B45" s="1">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" ref="C45:C64" si="2">C44+0.1</f>
-        <v>4.5999999999999996</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -981,11 +980,10 @@
         <v>3</v>
       </c>
       <c r="B46" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C46" s="1">
-        <f t="shared" si="2"/>
-        <v>4.6999999999999993</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -993,11 +991,11 @@
         <v>3</v>
       </c>
       <c r="B47" s="1">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" si="2"/>
-        <v>4.7999999999999989</v>
+        <f t="shared" ref="C47:C66" si="2">C46+0.1</f>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1005,11 +1003,11 @@
         <v>3</v>
       </c>
       <c r="B48" s="1">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C48" s="1">
         <f t="shared" si="2"/>
-        <v>4.8999999999999986</v>
+        <v>4.6999999999999993</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1017,11 +1015,11 @@
         <v>3</v>
       </c>
       <c r="B49" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.3</v>
       </c>
       <c r="C49" s="1">
         <f t="shared" si="2"/>
-        <v>4.9999999999999982</v>
+        <v>4.7999999999999989</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1029,11 +1027,11 @@
         <v>3</v>
       </c>
       <c r="B50" s="1">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="C50" s="1">
         <f t="shared" si="2"/>
-        <v>5.0999999999999979</v>
+        <v>4.8999999999999986</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1041,11 +1039,11 @@
         <v>3</v>
       </c>
       <c r="B51" s="1">
-        <v>0.85</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C51" s="1">
         <f t="shared" si="2"/>
-        <v>5.1999999999999975</v>
+        <v>4.9999999999999982</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1053,11 +1051,11 @@
         <v>3</v>
       </c>
       <c r="B52" s="1">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="C52" s="1">
         <f t="shared" si="2"/>
-        <v>5.2999999999999972</v>
+        <v>5.0999999999999979</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1065,11 +1063,11 @@
         <v>3</v>
       </c>
       <c r="B53" s="1">
-        <v>1.1499999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="C53" s="1">
         <f t="shared" si="2"/>
-        <v>5.3999999999999968</v>
+        <v>5.1999999999999975</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1077,11 +1075,11 @@
         <v>3</v>
       </c>
       <c r="B54" s="1">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="C54" s="1">
         <f t="shared" si="2"/>
-        <v>5.4999999999999964</v>
+        <v>5.2999999999999972</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1089,11 +1087,11 @@
         <v>3</v>
       </c>
       <c r="B55" s="1">
-        <v>1.48</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C55" s="1">
         <f t="shared" si="2"/>
-        <v>5.5999999999999961</v>
+        <v>5.3999999999999968</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1101,11 +1099,11 @@
         <v>3</v>
       </c>
       <c r="B56" s="1">
-        <v>1.64</v>
+        <v>1.3</v>
       </c>
       <c r="C56" s="1">
         <f t="shared" si="2"/>
-        <v>5.6999999999999957</v>
+        <v>5.4999999999999964</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1113,11 +1111,11 @@
         <v>3</v>
       </c>
       <c r="B57" s="1">
-        <v>1.8</v>
+        <v>1.48</v>
       </c>
       <c r="C57" s="1">
         <f t="shared" si="2"/>
-        <v>5.7999999999999954</v>
+        <v>5.5999999999999961</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1125,11 +1123,11 @@
         <v>3</v>
       </c>
       <c r="B58" s="1">
-        <v>1.96</v>
+        <v>1.64</v>
       </c>
       <c r="C58" s="1">
         <f t="shared" si="2"/>
-        <v>5.899999999999995</v>
+        <v>5.6999999999999957</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1137,11 +1135,11 @@
         <v>3</v>
       </c>
       <c r="B59" s="1">
-        <v>2.17</v>
+        <v>1.8</v>
       </c>
       <c r="C59" s="1">
         <f t="shared" si="2"/>
-        <v>5.9999999999999947</v>
+        <v>5.7999999999999954</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1149,11 +1147,11 @@
         <v>3</v>
       </c>
       <c r="B60" s="1">
-        <v>2.35</v>
+        <v>1.96</v>
       </c>
       <c r="C60" s="1">
         <f t="shared" si="2"/>
-        <v>6.0999999999999943</v>
+        <v>5.899999999999995</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1161,11 +1159,11 @@
         <v>3</v>
       </c>
       <c r="B61" s="1">
-        <v>2.58</v>
+        <v>2.17</v>
       </c>
       <c r="C61" s="1">
         <f t="shared" si="2"/>
-        <v>6.199999999999994</v>
+        <v>5.9999999999999947</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1173,11 +1171,11 @@
         <v>3</v>
       </c>
       <c r="B62" s="1">
-        <v>2.8</v>
+        <v>2.35</v>
       </c>
       <c r="C62" s="1">
         <f t="shared" si="2"/>
-        <v>6.2999999999999936</v>
+        <v>6.0999999999999943</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1185,11 +1183,11 @@
         <v>3</v>
       </c>
       <c r="B63" s="1">
-        <v>3.02</v>
+        <v>2.58</v>
       </c>
       <c r="C63" s="1">
         <f t="shared" si="2"/>
-        <v>6.3999999999999932</v>
+        <v>6.199999999999994</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1197,11 +1195,46 @@
         <v>3</v>
       </c>
       <c r="B64" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="C64" s="1">
+        <f t="shared" si="2"/>
+        <v>6.2999999999999936</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="1">
+        <v>3.02</v>
+      </c>
+      <c r="C65" s="1">
+        <f t="shared" si="2"/>
+        <v>6.3999999999999932</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="1">
         <v>3.3</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C66" s="1">
         <f t="shared" si="2"/>
         <v>6.4999999999999929</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" s="1">
+        <v>13</v>
+      </c>
+      <c r="C67" s="1">
+        <v>8.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>